<commit_message>
Stop Scanning after Result
Stop Scanning after Success, to prevent other pages to scan aswell
</commit_message>
<xml_diff>
--- a/docs/Projektanforderungen.xlsx
+++ b/docs/Projektanforderungen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\HTW\4Semester\ITProduction\App\worker_assistance_battery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedri\Documents\HTW\4Semester\ITProduction\App\worker_assistance_battery\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014A811D-DBC1-4478-ADCD-42B2B8100CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5821A3A-88E2-4C57-9664-8DDA4ABC5351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1EC2D5B-1EE7-4D48-8C10-9E2D0760D3BE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Anforderungsliste Worker Assistance Battery Projekt</t>
   </si>
@@ -59,9 +59,6 @@
     <t>P</t>
   </si>
   <si>
-    <t xml:space="preserve">Eine Mobile Anwendung für das Betriebssystem Android erstellen. </t>
-  </si>
-  <si>
     <t>Bauteil Scannen</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>Bemerkung</t>
   </si>
   <si>
-    <t>Grafiken aus 3D Druck anfragen</t>
-  </si>
-  <si>
     <t>Plattformunabhängigkeit</t>
   </si>
   <si>
@@ -126,6 +120,33 @@
   </si>
   <si>
     <t>Die Anwendung kann auf Android/iOS/Nexus Smartphone/Tablet installiert und ausgeführt werden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eine Webserver und Mobile Anwendung für das Betriebssystem Android erstellen. </t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>ToDo</t>
+  </si>
+  <si>
+    <t>Schritte ausformulieren und vorher/nachher Bilder hinzufügen</t>
+  </si>
+  <si>
+    <t>UI Kontrollieren, Bilder gleich groß</t>
+  </si>
+  <si>
+    <t>In WorkflowStep description_detail_german und englisch hinzufügen, damit später geswitched werden kann</t>
+  </si>
+  <si>
+    <t>Bilder selbst machen und Hintergrund entfernen</t>
+  </si>
+  <si>
+    <t>Wenn Zeit am Ende, eher nicht</t>
   </si>
 </sst>
 </file>
@@ -213,13 +234,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -554,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F6D6C5-4117-47AC-8641-AE9B2899D72C}">
-  <dimension ref="B2:F22"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,15 +588,16 @@
     <col min="3" max="3" width="32.44140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="78.77734375" customWidth="1"/>
-    <col min="6" max="6" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.88671875" customWidth="1"/>
+    <col min="8" max="8" width="87.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
@@ -587,10 +611,16 @@
         <v>4</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -601,198 +631,252 @@
         <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>